<commit_message>
Correct output files with 2018 and trying to add lines to plots
</commit_message>
<xml_diff>
--- a/Output_Files/20240826_DischargeSlope_FullFunctional.xlsx
+++ b/Output_Files/20240826_DischargeSlope_FullFunctional.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -620,47 +620,47 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>LOC_2019</t>
+          <t>LOC_2018</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2019-04-23</t>
+          <t>2018-05-01</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2019-05-28</t>
+          <t>2018-05-07</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>227.33</t>
+          <t>249.24</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>368.62</t>
+          <t>274.43</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.981771912766996</t>
+          <t>0.994623944470636</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3.71002963549723e-31</t>
+          <t>7.20898114739464e-07</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4.77391379474699e-05</t>
+          <t>4.62177579364686e-05</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>-74059.5116702037</t>
+          <t>-70239.7286160114</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -672,47 +672,47 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>LOC_2020</t>
+          <t>LOC_2019</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2020-04-28</t>
+          <t>2019-04-23</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>2020-05-04</t>
+          <t>2019-05-28</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>84.9800000000001</t>
+          <t>227.33</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>116.53</t>
+          <t>368.62</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.90471719099488</t>
+          <t>0.981771912766996</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0.000985819270105097</t>
+          <t>3.71002963549723e-31</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>6.18716931216247e-05</t>
+          <t>4.77391379474699e-05</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>-98175.6905951294</t>
+          <t>-74059.5116702037</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -724,47 +724,47 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOC_2021</t>
+          <t>LOC_2020</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2021-04-27</t>
+          <t>2020-04-28</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2021-05-24</t>
+          <t>2020-05-04</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>56.79</t>
+          <t>84.9800000000001</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>227.04</t>
+          <t>116.53</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.804633019960224</t>
+          <t>0.90471719099488</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>1.03478752047711e-10</t>
+          <t>0.000985819270105097</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>5.87799202801587e-05</t>
+          <t>6.18716931216247e-05</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>-95161.2197104754</t>
+          <t>-98175.6905951294</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -776,47 +776,47 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>LOC_2022</t>
+          <t>LOC_2021</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2022-05-03</t>
+          <t>2021-04-27</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2022-05-16</t>
+          <t>2021-05-24</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>91.88</t>
+          <t>56.79</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>157.23</t>
+          <t>227.04</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.947674675873266</t>
+          <t>0.804633019960224</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>4.73756615766804e-09</t>
+          <t>1.03478752047711e-10</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>5.51279507529542e-05</t>
+          <t>5.87799202801587e-05</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>-90962.0107848042</t>
+          <t>-95161.2197104754</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -828,50 +828,102 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>LOC_2022</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2022-05-03</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2022-05-16</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>91.88</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>157.23</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>0.947674675873266</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>4.73756615766804e-09</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>5.51279507529542e-05</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>-90962.0107848042</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>full_ice_to_functional_ice_off</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>LOC_2023</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B11" t="inlineStr">
         <is>
           <t>2023-05-02</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>2023-05-15</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>109.85</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>165.24</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>0.973869050019307</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>7.26380103121351e-11</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>4.277574277576e-05</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>-71882.1842124833</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>full_ice_to_functional_ice_off</t>
         </is>

</xml_diff>